<commit_message>
Melanie |#0000|Adding Ft for datetime and or-other
</commit_message>
<xml_diff>
--- a/func_tests/tests/advancedquestionnairetests/testdata/image.xlsx
+++ b/func_tests/tests/advancedquestionnairetests/testdata/image.xlsx
@@ -5,17 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="340" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="199" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="choices" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>type</t>
   </si>
@@ -36,6 +37,30 @@
   </si>
   <si>
     <t>text</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>select_multiple select_list or_other</t>
+  </si>
+  <si>
+    <t>selectOneQuestion</t>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>select_list</t>
+  </si>
+  <si>
+    <t>option_list1</t>
+  </si>
+  <si>
+    <t>option_list2</t>
   </si>
 </sst>
 </file>
@@ -146,7 +171,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
@@ -155,6 +180,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="6" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -235,14 +261,14 @@
   <dimension ref="A1:M87"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100">
-      <selection activeCell="C3" activeCellId="0" pane="topLeft" sqref="C3"/>
+      <selection activeCell="A5" activeCellId="0" pane="topLeft" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1764705882353"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.91764705882353"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.4980392156863"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.91764705882353"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.8666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3019607843137"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.643137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.0078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1" s="2">
@@ -288,8 +314,28 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="24" outlineLevel="0" r="4" s="3"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="84" outlineLevel="0" r="5"/>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="24" outlineLevel="0" r="4" s="3">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="84" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="6"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="7"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="8"/>
@@ -381,4 +427,65 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
+      <c r="A1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
+      <c r="A2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
+      <c r="A3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>